<commit_message>
Started creating figures for mtg 20200129
</commit_message>
<xml_diff>
--- a/data/scutellariaList.xlsx
+++ b/data/scutellariaList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B98E23-37C1-48CF-8289-CC89C3B965D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97FCEF6-6992-4779-A3F3-532E657A4E7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{D81E299B-7B47-4EAF-8A60-AAE40AE3D000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="150">
   <si>
     <t>Name</t>
   </si>
@@ -123,9 +123,6 @@
     <t>YH 2019-08-13</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Seed count</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t>frozenseeds.com</t>
   </si>
   <si>
-    <t>SLAT003-2</t>
-  </si>
-  <si>
     <t>SBAR 002</t>
   </si>
   <si>
@@ -373,6 +367,123 @@
   </si>
   <si>
     <t>fructicosa</t>
+  </si>
+  <si>
+    <t>SLAT 003-2</t>
+  </si>
+  <si>
+    <t>Old code</t>
+  </si>
+  <si>
+    <t>New code</t>
+  </si>
+  <si>
+    <t>ALP 000</t>
+  </si>
+  <si>
+    <t>GAL 000</t>
+  </si>
+  <si>
+    <t>HAS 000</t>
+  </si>
+  <si>
+    <t>ALT 000</t>
+  </si>
+  <si>
+    <t>ARE 000</t>
+  </si>
+  <si>
+    <t>BAR 000</t>
+  </si>
+  <si>
+    <t>HAV 000</t>
+  </si>
+  <si>
+    <t>INC 000</t>
+  </si>
+  <si>
+    <t>IND 000</t>
+  </si>
+  <si>
+    <t>INT 000</t>
+  </si>
+  <si>
+    <t>LAT 000</t>
+  </si>
+  <si>
+    <t>BAI 000</t>
+  </si>
+  <si>
+    <t>BAI 001</t>
+  </si>
+  <si>
+    <t>BAI 002</t>
+  </si>
+  <si>
+    <t>BAR 002</t>
+  </si>
+  <si>
+    <t>BAR 001</t>
+  </si>
+  <si>
+    <t>GAL 001</t>
+  </si>
+  <si>
+    <t>HAS 001</t>
+  </si>
+  <si>
+    <t>BAR 003</t>
+  </si>
+  <si>
+    <t>LAT 003</t>
+  </si>
+  <si>
+    <t>BAR 004</t>
+  </si>
+  <si>
+    <t>BAR 005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAT 001 </t>
+  </si>
+  <si>
+    <t>LAT 002</t>
+  </si>
+  <si>
+    <t>LEO 000</t>
+  </si>
+  <si>
+    <t>LEO 001</t>
+  </si>
+  <si>
+    <t>LEO 002</t>
+  </si>
+  <si>
+    <t>OVA 000</t>
+  </si>
+  <si>
+    <t>OVA 001</t>
+  </si>
+  <si>
+    <t>RAC-MS 000</t>
+  </si>
+  <si>
+    <t>RAC-MS 001</t>
+  </si>
+  <si>
+    <t>RAC-MS 002</t>
+  </si>
+  <si>
+    <t>RAC-MS 003</t>
+  </si>
+  <si>
+    <t>RAC-SC 000</t>
+  </si>
+  <si>
+    <t>RAC-SC 001</t>
+  </si>
+  <si>
+    <t>TOU 000</t>
   </si>
 </sst>
 </file>
@@ -420,11 +531,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -756,12 +867,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
         <v>17</v>
@@ -1196,7 +1307,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1206,132 +1317,132 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1344,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF67D2B-BFB7-4490-9B6D-4F3EF1324AEE}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,520 +1469,631 @@
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="2">
+        <v>43565</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="2">
+        <v>43779</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="2">
+        <v>43686</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="2">
+        <v>43656</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="2">
+        <v>43409</v>
+      </c>
+      <c r="E15" s="3">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17" s="2">
+        <v>43565</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="3">
+        <v>50</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" s="3">
+        <v>20</v>
+      </c>
+      <c r="F19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="2">
+        <v>43411</v>
+      </c>
+      <c r="E20" s="3">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="2">
+        <v>43405</v>
+      </c>
+      <c r="E22" s="3">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="2">
+        <v>43580</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="2">
+        <v>43565</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="2">
+        <v>43409</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>141</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="2">
+        <v>43403</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" s="2">
+        <v>43588</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="2">
+        <v>43656</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" s="2">
+        <v>43592</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="2">
+        <v>43739</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" s="2">
+        <v>43656</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36" s="2">
+        <v>43592</v>
+      </c>
+      <c r="E36" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="2">
-        <v>43565</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="2">
-        <v>43779</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="2">
-        <v>43686</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="2">
-        <v>43656</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="2">
-        <v>43409</v>
-      </c>
-      <c r="D15" s="4">
-        <v>20</v>
-      </c>
-      <c r="E15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="2">
-        <v>43565</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="4">
-        <v>50</v>
-      </c>
-      <c r="E18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="4">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="2">
-        <v>43411</v>
-      </c>
-      <c r="D20" s="4">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="2">
-        <v>43405</v>
-      </c>
-      <c r="D22" s="4">
-        <v>25</v>
-      </c>
-      <c r="E22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="2">
-        <v>43580</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="2">
-        <v>43565</v>
-      </c>
-      <c r="D26" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="2">
-        <v>43409</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0</v>
-      </c>
-      <c r="E28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0</v>
-      </c>
-      <c r="E29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="2">
-        <v>43403</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="2">
-        <v>43588</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="2">
-        <v>43656</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="2">
-        <v>43592</v>
-      </c>
-      <c r="D33" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="2">
-        <v>43739</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="2">
-        <v>43656</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="2">
-        <v>43592</v>
-      </c>
-      <c r="D36" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="E38" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="4">
-        <v>0</v>
-      </c>
-      <c r="E37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>74</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>37</v>
+      <c r="E39" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed several errors in figure legend
</commit_message>
<xml_diff>
--- a/data/scutellariaList.xlsx
+++ b/data/scutellariaList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D77E65-5ABE-4287-B65D-F2AF67FA498B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A911C489-8313-4FD2-8BD8-1B9FF1866A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{D81E299B-7B47-4EAF-8A60-AAE40AE3D000}"/>
   </bookViews>
@@ -1012,13 +1012,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1033,6 +1027,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,12 +1364,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -3298,8 +3298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACB3469-65F3-498A-B152-2C62F11F4B84}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3309,940 +3309,940 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="B5" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+      <c r="B6" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="B7" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
+      <c r="B8" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="B14" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="B15" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
+      <c r="B16" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="B19" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="8"/>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
+      <c r="B21" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
+      <c r="B22" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
+      <c r="B23" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="B24" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C25" s="9" t="s">
+      <c r="B25" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D25" s="10"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="B26" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="D26" s="8"/>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C27" s="9" t="s">
+      <c r="B27" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
+      <c r="B28" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="B29" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="B31" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="9" t="s">
+      <c r="A32" s="13"/>
+      <c r="B32" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="8"/>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
+      <c r="B33" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
+      <c r="B34" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
+      <c r="B35" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C36" s="9" t="s">
+      <c r="B36" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D36" s="10"/>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C37" s="9" t="s">
+      <c r="B37" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D37" s="10"/>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
+      <c r="B38" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D39" s="10"/>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D40" s="10"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
+      <c r="B41" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C42" s="9" t="s">
+      <c r="B42" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D42" s="10"/>
+      <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
+      <c r="B43" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
+      <c r="B44" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="B45" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C45" s="9" t="s">
+      <c r="B45" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="10"/>
+      <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="9" t="s">
+      <c r="A46" s="13"/>
+      <c r="B46" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D46" s="10"/>
+      <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="B47" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
+      <c r="B47" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
-      <c r="B48" s="9" t="s">
+      <c r="A48" s="13"/>
+      <c r="B48" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D48" s="10"/>
+      <c r="D48" s="8"/>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
+      <c r="B49" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C50" s="9" t="s">
+      <c r="B50" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D50" s="10"/>
+      <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
+      <c r="B51" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="B52" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C52" s="9" t="s">
+      <c r="B52" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D52" s="10"/>
+      <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="B53" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C53" s="9" t="s">
+      <c r="B53" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D53" s="10"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
+      <c r="B54" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="B55" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
+      <c r="B55" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="B56" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
+      <c r="B56" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="B57" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
+      <c r="B57" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B58" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
+      <c r="B58" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="B59" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C59" s="9" t="s">
+      <c r="B59" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C59" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D59" s="10"/>
+      <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B60" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C60" s="9" t="s">
+      <c r="B60" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="10"/>
+      <c r="D60" s="8"/>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="B61" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C61" s="9" t="s">
+      <c r="B61" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D61" s="10"/>
+      <c r="D61" s="8"/>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
+      <c r="A62" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="B62" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
+      <c r="B62" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D63" s="10"/>
+      <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="8" t="s">
+      <c r="A64" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="B64" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
+      <c r="B64" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="B65" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
+      <c r="B65" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
+      <c r="A66" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="B66" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C66" s="9" t="s">
+      <c r="B66" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C66" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D66" s="10"/>
+      <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
+      <c r="A67" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="B67" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
+      <c r="B67" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="B68" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
+      <c r="B68" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
+      <c r="A69" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="B69" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
+      <c r="B69" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
+      <c r="A70" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="B70" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C70" s="9" t="s">
+      <c r="B70" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C70" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D70" s="10"/>
+      <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
+      <c r="A71" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="B71" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
+      <c r="B71" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
+      <c r="A72" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="B72" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
+      <c r="B72" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
-      <c r="B73" s="9" t="s">
+      <c r="A73" s="13"/>
+      <c r="B73" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D73" s="10"/>
+      <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="B74" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
+      <c r="B74" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="B75" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C75" s="9" t="s">
+      <c r="B75" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C75" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D75" s="10"/>
+      <c r="D75" s="8"/>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
+      <c r="A76" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="B76" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C76" s="9" t="s">
+      <c r="B76" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C76" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D76" s="10"/>
+      <c r="D76" s="8"/>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="B77" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
+      <c r="B77" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
+      <c r="A78" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="B78" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
+      <c r="B78" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="B79" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C79" s="9" t="s">
+      <c r="B79" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C79" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D79" s="10"/>
+      <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="8" t="s">
+      <c r="A80" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="B80" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C80" s="9" t="s">
+      <c r="B80" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C80" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D80" s="10"/>
+      <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="B81" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C81" s="9" t="s">
+      <c r="B81" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C81" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D81" s="10"/>
+      <c r="D81" s="8"/>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B82" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C82" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D82" s="10"/>
+      <c r="D82" s="8"/>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="B83" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
+      <c r="B83" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
+      <c r="A84" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="B84" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
+      <c r="B84" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="8" t="s">
+      <c r="A85" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="B85" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C85" s="9" t="s">
+      <c r="B85" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C85" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D85" s="10"/>
+      <c r="D85" s="8"/>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="8" t="s">
+      <c r="A86" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B86" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="C86" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D86" s="10"/>
+      <c r="D86" s="8"/>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D87" s="5"/>

</xml_diff>

<commit_message>
Added flower photos and updated figure legend
</commit_message>
<xml_diff>
--- a/data/scutellariaList.xlsx
+++ b/data/scutellariaList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A911C489-8313-4FD2-8BD8-1B9FF1866A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905C6F57-455A-4628-96CA-1215ED9571D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{D81E299B-7B47-4EAF-8A60-AAE40AE3D000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="296">
   <si>
     <t>Name</t>
   </si>
@@ -911,13 +911,25 @@
   </si>
   <si>
     <t>S. tournefortii</t>
+  </si>
+  <si>
+    <t>Herbarium</t>
+  </si>
+  <si>
+    <t>Voucher #</t>
+  </si>
+  <si>
+    <t>Steere herbarium, NY, USA</t>
+  </si>
+  <si>
+    <t>UF herbarium, FL, USA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -932,11 +944,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -965,6 +972,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -999,7 +1020,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1009,30 +1030,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,12 +1391,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -3296,971 +3323,1397 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACB3469-65F3-498A-B152-2C62F11F4B84}">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I79" sqref="I79"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="4" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B28" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="E28" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="7" t="s">
+      <c r="E46" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="12"/>
+      <c r="C47" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D47" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="7" t="s">
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="12"/>
+      <c r="C49" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D49" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D50" s="7"/>
+      <c r="E50" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="E51" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D56" s="7"/>
+      <c r="E56" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D58" s="7"/>
+      <c r="E58" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C64" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D64" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="E64" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D65" s="7"/>
+      <c r="E65" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D66" s="7"/>
+      <c r="E66" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D68" s="7"/>
+      <c r="E68" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D69" s="7"/>
+      <c r="E69" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D70" s="7"/>
+      <c r="E70" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D72" s="7"/>
+      <c r="E72" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D73" s="7"/>
+      <c r="E73" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="12"/>
+      <c r="C74" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D74" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="E74" s="10"/>
+    </row>
+    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D75" s="7"/>
+      <c r="E75" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D78" s="7"/>
+      <c r="E78" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D79" s="7"/>
+      <c r="E79" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D80" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="E80" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D81" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B20" s="7" t="s">
+      <c r="E81" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C83" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D83" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C24" s="7" t="s">
+      <c r="E83" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D84" s="7"/>
+      <c r="E84" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D85" s="7"/>
+      <c r="E85" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D86" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="B30" s="7" t="s">
+      <c r="E86" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="C87" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="D87" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D36" s="8"/>
-    </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D37" s="8"/>
-    </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-    </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D39" s="8"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D40" s="8"/>
-    </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-    </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D42" s="8"/>
-    </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-    </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-    </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="8"/>
-    </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D46" s="8"/>
-    </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-    </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D48" s="8"/>
-    </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-    </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D50" s="8"/>
-    </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-    </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D52" s="8"/>
-    </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D53" s="8"/>
-    </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-    </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-    </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-    </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-    </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-    </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D59" s="8"/>
-    </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" s="8"/>
-    </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D61" s="8"/>
-    </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-    </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D63" s="8"/>
-    </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-    </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-    </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D66" s="8"/>
-    </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-    </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-    </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-    </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D70" s="8"/>
-    </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-    </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-    </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="B73" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D73" s="8"/>
-    </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-    </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D75" s="8"/>
-    </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D76" s="8"/>
-    </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-    </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-    </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="8"/>
-    </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D80" s="8"/>
-    </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D81" s="8"/>
-    </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D82" s="8"/>
-    </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-    </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-    </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D85" s="8"/>
-    </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D86" s="8"/>
-    </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D87" s="5"/>
-    </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D88" s="5"/>
+      <c r="E87" s="10"/>
+    </row>
+    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E88" s="15"/>
+    </row>
+    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E89" s="15"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D86">
-    <sortCondition ref="A2:A86"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E87">
+    <sortCondition ref="B2:B87"/>
   </sortState>
-  <mergeCells count="6">
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A45:A46"/>
+  <mergeCells count="7">
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="25" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added photos for wrightii and suffretescens
</commit_message>
<xml_diff>
--- a/data/scutellariaList.xlsx
+++ b/data/scutellariaList.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0289BA73-BA10-41FB-B8B2-058398D6A03E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2718994C-44FA-48F1-8958-33F64CA9CA80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{D81E299B-7B47-4EAF-8A60-AAE40AE3D000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{D81E299B-7B47-4EAF-8A60-AAE40AE3D000}"/>
   </bookViews>
   <sheets>
     <sheet name="samplesAnalyzed" sheetId="1" r:id="rId1"/>
     <sheet name="seedStock" sheetId="2" r:id="rId2"/>
     <sheet name="TableS1" sheetId="3" r:id="rId3"/>
+    <sheet name="vouchersToSubmit" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="436">
   <si>
     <t>Name</t>
   </si>
@@ -1491,7 +1492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1524,15 +1525,21 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1864,12 +1871,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -3798,8 +3805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACB3469-65F3-498A-B152-2C62F11F4B84}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3871,7 +3878,7 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="18" t="s">
         <v>215</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -3898,7 +3905,7 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="10" t="s">
         <v>206</v>
       </c>
@@ -4018,7 +4025,7 @@
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="18" t="s">
         <v>220</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -4038,7 +4045,7 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="10" t="s">
         <v>206</v>
       </c>
@@ -4107,7 +4114,7 @@
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="18" t="s">
         <v>223</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -4129,7 +4136,7 @@
       <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="10" t="s">
         <v>206</v>
       </c>
@@ -4557,7 +4564,7 @@
       <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="18" t="s">
         <v>239</v>
       </c>
       <c r="C31" s="10" t="s">
@@ -4582,7 +4589,7 @@
       <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="15"/>
+      <c r="B32" s="18"/>
       <c r="C32" s="10" t="s">
         <v>206</v>
       </c>
@@ -4901,7 +4908,7 @@
       <c r="A45" s="5">
         <v>44</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="18" t="s">
         <v>250</v>
       </c>
       <c r="C45" s="10" t="s">
@@ -4928,7 +4935,7 @@
       <c r="A46" s="5">
         <v>45</v>
       </c>
-      <c r="B46" s="15"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="10" t="s">
         <v>206</v>
       </c>
@@ -4948,7 +4955,7 @@
       <c r="A47" s="5">
         <v>46</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="18" t="s">
         <v>251</v>
       </c>
       <c r="C47" s="10" t="s">
@@ -4973,7 +4980,7 @@
       <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="15"/>
+      <c r="B48" s="18"/>
       <c r="C48" s="10" t="s">
         <v>206</v>
       </c>
@@ -5578,7 +5585,7 @@
       <c r="A72" s="5">
         <v>71</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B72" s="18" t="s">
         <v>273</v>
       </c>
       <c r="C72" s="10" t="s">
@@ -5598,7 +5605,7 @@
       <c r="A73" s="5">
         <v>72</v>
       </c>
-      <c r="B73" s="15"/>
+      <c r="B73" s="18"/>
       <c r="C73" s="10" t="s">
         <v>206</v>
       </c>
@@ -5951,13 +5958,13 @@
       <c r="F87"/>
     </row>
     <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="16" t="s">
+      <c r="B88" s="15" t="s">
         <v>433</v>
       </c>
-      <c r="C88" s="17" t="s">
+      <c r="C88" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="D88" s="17" t="s">
+      <c r="D88" s="16" t="s">
         <v>212</v>
       </c>
       <c r="E88" s="12" t="s">
@@ -5966,13 +5973,13 @@
       <c r="F88"/>
     </row>
     <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="16" t="s">
+      <c r="B89" s="15" t="s">
         <v>434</v>
       </c>
-      <c r="C89" s="17" t="s">
+      <c r="C89" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="D89" s="17" t="s">
+      <c r="D89" s="16" t="s">
         <v>212</v>
       </c>
       <c r="E89" s="12" t="s">
@@ -5980,10 +5987,10 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="16" t="s">
+      <c r="B90" s="15" t="s">
         <v>435</v>
       </c>
-      <c r="C90" s="17" t="s">
+      <c r="C90" s="16" t="s">
         <v>207</v>
       </c>
     </row>
@@ -6003,4 +6010,209 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="25" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D76920-7A5A-4925-A59B-3FCF8C196BA4}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="42" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>433</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added wrightii data and voucher photos
</commit_message>
<xml_diff>
--- a/data/scutellariaList.xlsx
+++ b/data/scutellariaList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2718994C-44FA-48F1-8958-33F64CA9CA80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA879AE-006B-44E6-AEE9-D84CC6E3E800}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{D81E299B-7B47-4EAF-8A60-AAE40AE3D000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{D81E299B-7B47-4EAF-8A60-AAE40AE3D000}"/>
   </bookViews>
   <sheets>
     <sheet name="samplesAnalyzed" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="436">
   <si>
     <t>Name</t>
   </si>
@@ -1532,14 +1532,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1871,12 +1871,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -2899,8 +2899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF67D2B-BFB7-4490-9B6D-4F3EF1324AEE}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3878,7 +3878,7 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>215</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -3905,7 +3905,7 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="10" t="s">
         <v>206</v>
       </c>
@@ -4025,7 +4025,7 @@
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="19" t="s">
         <v>220</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -4045,7 +4045,7 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="10" t="s">
         <v>206</v>
       </c>
@@ -4114,7 +4114,7 @@
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="19" t="s">
         <v>223</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -4136,7 +4136,7 @@
       <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="18"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="10" t="s">
         <v>206</v>
       </c>
@@ -4564,7 +4564,7 @@
       <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="19" t="s">
         <v>239</v>
       </c>
       <c r="C31" s="10" t="s">
@@ -4589,7 +4589,7 @@
       <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="18"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="10" t="s">
         <v>206</v>
       </c>
@@ -4908,7 +4908,7 @@
       <c r="A45" s="5">
         <v>44</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="19" t="s">
         <v>250</v>
       </c>
       <c r="C45" s="10" t="s">
@@ -4935,7 +4935,7 @@
       <c r="A46" s="5">
         <v>45</v>
       </c>
-      <c r="B46" s="18"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="10" t="s">
         <v>206</v>
       </c>
@@ -4955,7 +4955,7 @@
       <c r="A47" s="5">
         <v>46</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="19" t="s">
         <v>251</v>
       </c>
       <c r="C47" s="10" t="s">
@@ -4980,7 +4980,7 @@
       <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="18"/>
+      <c r="B48" s="19"/>
       <c r="C48" s="10" t="s">
         <v>206</v>
       </c>
@@ -5585,7 +5585,7 @@
       <c r="A72" s="5">
         <v>71</v>
       </c>
-      <c r="B72" s="18" t="s">
+      <c r="B72" s="19" t="s">
         <v>273</v>
       </c>
       <c r="C72" s="10" t="s">
@@ -5605,7 +5605,7 @@
       <c r="A73" s="5">
         <v>72</v>
       </c>
-      <c r="B73" s="18"/>
+      <c r="B73" s="19"/>
       <c r="C73" s="10" t="s">
         <v>206</v>
       </c>
@@ -6016,8 +6016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D76920-7A5A-4925-A59B-3FCF8C196BA4}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6055,7 +6055,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>215</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -6071,7 +6071,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>220</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -6103,23 +6103,15 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>394</v>
-      </c>
+      <c r="A5" s="15"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="17" t="s">
         <v>239</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -6135,23 +6127,15 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>250</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>394</v>
-      </c>
+      <c r="A7" s="17"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="17" t="s">
         <v>251</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -6167,7 +6151,7 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="17" t="s">
         <v>273</v>
       </c>
       <c r="B9" s="10" t="s">

</xml_diff>

<commit_message>
Updated figures and added wrightii data
</commit_message>
<xml_diff>
--- a/data/scutellariaList.xlsx
+++ b/data/scutellariaList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8183FD5C-6879-4986-A936-AB8EA741E4DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A6A719-AF3C-430F-A6E1-88904DD9675D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{D81E299B-7B47-4EAF-8A60-AAE40AE3D000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{D81E299B-7B47-4EAF-8A60-AAE40AE3D000}"/>
   </bookViews>
   <sheets>
     <sheet name="samplesAnalyzed" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="456">
   <si>
     <t>Name</t>
   </si>
@@ -689,9 +689,6 @@
     <t>S. angulosa</t>
   </si>
   <si>
-    <t>S. angustifolia ssp. angustifolia</t>
-  </si>
-  <si>
     <t>S. angustifolia ssp. micrathum</t>
   </si>
   <si>
@@ -758,9 +755,6 @@
     <t>S. havanensis</t>
   </si>
   <si>
-    <t>S. heterophylla</t>
-  </si>
-  <si>
     <t>S. heydei</t>
   </si>
   <si>
@@ -773,9 +767,6 @@
     <t>S. hookeri</t>
   </si>
   <si>
-    <t>S. incanca</t>
-  </si>
-  <si>
     <t>S. insignis</t>
   </si>
   <si>
@@ -1008,12 +999,6 @@
   </si>
   <si>
     <t>J. K. Small s. n.</t>
-  </si>
-  <si>
-    <t>NYBG62</t>
-  </si>
-  <si>
-    <t>A. Bertschinger s. n.</t>
   </si>
   <si>
     <t>NYBG63</t>
@@ -1386,12 +1371,6 @@
     <t>S. wrightii</t>
   </si>
   <si>
-    <t>S. suffretescens</t>
-  </si>
-  <si>
-    <t>S. suffretescens x resinosa</t>
-  </si>
-  <si>
     <t>LEO 003</t>
   </si>
   <si>
@@ -1426,6 +1405,51 @@
   </si>
   <si>
     <t>WRI 001</t>
+  </si>
+  <si>
+    <t>S. angustifolia</t>
+  </si>
+  <si>
+    <t>FLAS01</t>
+  </si>
+  <si>
+    <t>Paul Corogin SB104</t>
+  </si>
+  <si>
+    <t>Stem</t>
+  </si>
+  <si>
+    <t>FLAS02</t>
+  </si>
+  <si>
+    <t>D. B. Wand 6711</t>
+  </si>
+  <si>
+    <t>FLAS04</t>
+  </si>
+  <si>
+    <t>Nancy Coile 5213</t>
+  </si>
+  <si>
+    <t>S. incana</t>
+  </si>
+  <si>
+    <t>FLAS05</t>
+  </si>
+  <si>
+    <t>Kimberely Gulledge 25</t>
+  </si>
+  <si>
+    <t>FLAS06</t>
+  </si>
+  <si>
+    <t>Hillary M. Cherry 270</t>
+  </si>
+  <si>
+    <t>FLAS07</t>
+  </si>
+  <si>
+    <t>s. n.</t>
   </si>
 </sst>
 </file>
@@ -1493,18 +1517,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1528,7 +1546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1554,13 +1572,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1571,11 +1585,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1893,7 +1914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B26A3BC-753B-4215-92EB-E0126892F519}">
   <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1907,12 +1928,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -2935,7 +2956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF67D2B-BFB7-4490-9B6D-4F3EF1324AEE}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -3623,7 +3644,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
@@ -3637,7 +3658,7 @@
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="D42" s="2">
         <v>44104</v>
@@ -3747,7 +3768,7 @@
         <v>36</v>
       </c>
       <c r="C49" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="D49" s="2">
         <v>44104</v>
@@ -3756,7 +3777,7 @@
         <v>32</v>
       </c>
       <c r="F49" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3792,10 +3813,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="C52" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="D52" s="2">
         <v>44104</v>
@@ -3804,15 +3825,15 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="C53" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="D53" s="2">
         <v>44104</v>
@@ -3821,7 +3842,7 @@
         <v>32</v>
       </c>
       <c r="F53" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3894,10 +3915,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="C58" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="D58" s="2">
         <v>44089</v>
@@ -3906,15 +3927,15 @@
         <v>32</v>
       </c>
       <c r="F58" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="C59" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="D59" s="2">
         <v>44104</v>
@@ -3923,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -3952,10 +3973,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACB3469-65F3-498A-B152-2C62F11F4B84}">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3972,7 +3993,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>210</v>
@@ -3984,23 +4005,23 @@
         <v>211</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="16" t="s">
         <v>214</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -4010,13 +4031,13 @@
         <v>213</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H2" t="str">
         <f>IF(E2="Steere Herbarium, NY, USA", CONCATENATE(G2, " (NY)"), IF(E2="University of Florida Herbarium, FL, USA", CONCATENATE(G2, " (FLAS)"), IF(E2="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G2, " (SWU)"), "Herbarium name not recognized")))</f>
@@ -4027,7 +4048,7 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>215</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -4037,16 +4058,16 @@
         <v>4</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H66" si="0">IF(E3="Steere Herbarium, NY, USA", CONCATENATE(G3, " (NY)"), IF(E3="University of Florida Herbarium, FL, USA", CONCATENATE(G3, " (FLAS)"), IF(E3="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G3, " (SWU)"), "Herbarium name not recognized")))</f>
+        <f t="shared" ref="H3:H64" si="0">IF(E3="Steere Herbarium, NY, USA", CONCATENATE(G3, " (NY)"), IF(E3="University of Florida Herbarium, FL, USA", CONCATENATE(G3, " (FLAS)"), IF(E3="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G3, " (SWU)"), "Herbarium name not recognized")))</f>
         <v>M. Churadze 1007 (NY)</v>
       </c>
     </row>
@@ -4054,15 +4075,15 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="10" t="s">
         <v>206</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>424</v>
+      <c r="E4" s="11" t="s">
+        <v>419</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" t="str">
@@ -4074,21 +4095,23 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="16" t="s">
         <v>216</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E5" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -4099,21 +4122,23 @@
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>217</v>
+      <c r="B6" s="16" t="s">
+        <v>441</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E6" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -4124,21 +4149,23 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>218</v>
+      <c r="B7" s="16" t="s">
+        <v>217</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E7" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -4149,24 +4176,26 @@
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>219</v>
+      <c r="B8" s="16" t="s">
+        <v>218</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E8" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(E8="Steere Herbarium, NY, USA", CONCATENATE(G8, " (NY)"), IF(E8="University of Florida Herbarium, FL, USA", CONCATENATE(G8, " (FLAS)"), IF(E8="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G8, " (SWU)"), "Herbarium name not recognized")))</f>
         <v>N. D. Atwood 28625 (NY)</v>
       </c>
     </row>
@@ -4174,97 +4203,107 @@
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="G9" s="13"/>
+      <c r="B9" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>443</v>
+      </c>
       <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> (FLAS)</v>
+        <f t="shared" ref="H9" si="1">IF(E9="Steere Herbarium, NY, USA", CONCATENATE(G9, " (NY)"), IF(E9="University of Florida Herbarium, FL, USA", CONCATENATE(G9, " (FLAS)"), IF(E9="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G9, " (SWU)"), "Herbarium name not recognized")))</f>
+        <v>Paul Corogin SB104 (FLAS)</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="G10" s="5"/>
+        <v>207</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>446</v>
+      </c>
       <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>Herbarium name not recognized</v>
+        <f>IF(E10="Steere Herbarium, NY, USA", CONCATENATE(G10, " (NY)"), IF(E10="University of Florida Herbarium, FL, USA", CONCATENATE(G10, " (FLAS)"), IF(E10="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G10, " (SWU)"), "Herbarium name not recognized")))</f>
+        <v>D. B. Wand 6711 (FLAS)</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>221</v>
-      </c>
+      <c r="B11" s="18"/>
       <c r="C11" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>399</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="G11" s="5"/>
       <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>J. T. Howell 38532 (NY)</v>
+        <f>IF(E11="Steere Herbarium, NY, USA", CONCATENATE(G11, " (NY)"), IF(E11="University of Florida Herbarium, FL, USA", CONCATENATE(G11, " (FLAS)"), IF(E11="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G11, " (SWU)"), "Herbarium name not recognized")))</f>
+        <v>Herbarium name not recognized</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>222</v>
+      <c r="B12" s="16" t="s">
+        <v>220</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="G12" s="5"/>
+        <v>213</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>394</v>
+      </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>Herbarium name not recognized</v>
+        <v>J. T. Howell 38532 (NY)</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>223</v>
+      <c r="B13" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>206</v>
@@ -4272,8 +4311,8 @@
       <c r="D13" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>424</v>
+      <c r="E13" s="11" t="s">
+        <v>419</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" t="str">
@@ -4285,7 +4324,9 @@
       <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="15" t="s">
+        <v>222</v>
+      </c>
       <c r="C14" s="10" t="s">
         <v>206</v>
       </c>
@@ -4293,10 +4334,10 @@
         <v>212</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -4307,21 +4348,23 @@
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>224</v>
+      <c r="B15" s="16" t="s">
+        <v>223</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>444</v>
+      </c>
       <c r="E15" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>395</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>400</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -4332,21 +4375,23 @@
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>225</v>
+      <c r="B16" s="16" t="s">
+        <v>224</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E16" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -4357,24 +4402,26 @@
       <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>226</v>
+      <c r="B17" s="16" t="s">
+        <v>225</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E17" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(E17="Steere Herbarium, NY, USA", CONCATENATE(G17, " (NY)"), IF(E17="University of Florida Herbarium, FL, USA", CONCATENATE(G17, " (FLAS)"), IF(E17="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G17, " (SWU)"), "Herbarium name not recognized")))</f>
         <v>R. Olmstead 434 (NY)</v>
       </c>
     </row>
@@ -4382,21 +4429,23 @@
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>227</v>
+      <c r="B18" s="16" t="s">
+        <v>226</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E18" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -4407,8 +4456,8 @@
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>228</v>
+      <c r="B19" s="16" t="s">
+        <v>227</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>207</v>
@@ -4417,13 +4466,13 @@
         <v>4</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -4434,8 +4483,8 @@
       <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>229</v>
+      <c r="B20" s="16" t="s">
+        <v>228</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>207</v>
@@ -4444,13 +4493,13 @@
         <v>213</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -4461,8 +4510,8 @@
       <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>230</v>
+      <c r="B21" s="16" t="s">
+        <v>229</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>206</v>
@@ -4471,10 +4520,10 @@
         <v>212</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -4485,21 +4534,23 @@
       <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>231</v>
+      <c r="B22" s="16" t="s">
+        <v>230</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E22" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -4510,21 +4561,23 @@
       <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>232</v>
+      <c r="B23" s="16" t="s">
+        <v>231</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="6" t="s">
+        <v>444</v>
+      </c>
       <c r="E23" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -4535,28 +4588,35 @@
       <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>233</v>
+      <c r="B24" s="16" t="s">
+        <v>232</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E24" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="G24" s="13"/>
+        <v>389</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>448</v>
+      </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (FLAS)</v>
+        <v>Nancy Coile 5213 (FLAS)</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>234</v>
+      <c r="B25" s="16" t="s">
+        <v>233</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>207</v>
@@ -4565,13 +4625,13 @@
         <v>213</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -4582,8 +4642,8 @@
       <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>235</v>
+      <c r="B26" s="16" t="s">
+        <v>234</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>207</v>
@@ -4592,13 +4652,13 @@
         <v>213</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -4609,8 +4669,8 @@
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>315</v>
+      <c r="B27" s="16" t="s">
+        <v>312</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>207</v>
@@ -4619,13 +4679,13 @@
         <v>4</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -4636,8 +4696,8 @@
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>236</v>
+      <c r="B28" s="16" t="s">
+        <v>235</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>207</v>
@@ -4646,13 +4706,13 @@
         <v>213</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -4663,21 +4723,23 @@
       <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>237</v>
+      <c r="B29" s="16" t="s">
+        <v>236</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E29" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -4688,21 +4750,23 @@
       <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>238</v>
+      <c r="B30" s="16" t="s">
+        <v>237</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>444</v>
+      </c>
       <c r="E30" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -4713,21 +4777,23 @@
       <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>239</v>
+      <c r="B31" s="18" t="s">
+        <v>238</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>444</v>
+      </c>
       <c r="E31" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -4738,15 +4804,15 @@
       <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="18"/>
       <c r="C32" s="10" t="s">
         <v>206</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E32" s="12" t="s">
-        <v>424</v>
+      <c r="E32" s="11" t="s">
+        <v>419</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" t="str">
@@ -4758,341 +4824,360 @@
       <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>240</v>
+      <c r="B33" s="16" t="s">
+        <v>239</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D33" s="10"/>
+      <c r="D33" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E33" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>325</v>
+        <v>402</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
-        <v>A. Bertschinger s. n. (NY)</v>
+        <v>W. Koelz 6242 (NY)</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>241</v>
+      <c r="B34" s="16" t="s">
+        <v>240</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D34" s="6"/>
+      <c r="D34" s="6" t="s">
+        <v>444</v>
+      </c>
       <c r="E34" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>407</v>
+        <v>323</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
-        <v>W. Koelz 6242 (NY)</v>
+        <v>R. D. Worthington 12501 (NY)</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="11" t="s">
-        <v>242</v>
+      <c r="B35" s="16" t="s">
+        <v>241</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D35" s="6"/>
+      <c r="D35" s="6" t="s">
+        <v>213</v>
+      </c>
       <c r="E35" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>328</v>
+        <v>403</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
-        <v>R. D. Worthington 12501 (NY)</v>
+        <v>G. Schoolcraft 1222 (NY)</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="11" t="s">
-        <v>243</v>
+      <c r="B36" s="16" t="s">
+        <v>242</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="10" t="s">
         <v>213</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>408</v>
+        <v>326</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
-        <v>G. Schoolcraft 1222 (NY)</v>
+        <v>L. O. Willioms et al. 28585 (NY)</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>244</v>
+      <c r="B37" s="16" t="s">
+        <v>449</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>207</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>213</v>
+        <v>4</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>331</v>
+        <v>404</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
-        <v>L. O. Willioms et al. 28585 (NY)</v>
+        <v>R. D. Thomas 150388 (NY)</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>245</v>
+      <c r="B38" s="16" t="s">
+        <v>425</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D38" s="10"/>
+        <v>206</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>212</v>
+      </c>
       <c r="E38" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>332</v>
+        <v>393</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>409</v>
+        <v>421</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
-        <v>R. D. Thomas 150388 (NY)</v>
+        <v>S. Kim &amp; S. T. Lee 2015-0298 (SWU)</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>430</v>
+      <c r="B39" s="16" t="s">
+        <v>243</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="10" t="s">
         <v>212</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
-        <v>S. Kim &amp; S. T. Lee 2015-0298 (SWU)</v>
+        <v>S. Kim 2015-0110 (SWU)</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>246</v>
+      <c r="B40" s="16" t="s">
+        <v>244</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>212</v>
+        <v>4</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>427</v>
+        <v>389</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>451</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
-        <v>S. Kim 2015-0110 (SWU)</v>
+        <v>Kimberely Gulledge 25 (FLAS)</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
-      <c r="B41" s="11" t="s">
-        <v>247</v>
+      <c r="B41" s="16" t="s">
+        <v>427</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D41" s="10"/>
+      <c r="D41" s="6" t="s">
+        <v>213</v>
+      </c>
       <c r="E41" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="G41" s="13"/>
+        <v>390</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>405</v>
+      </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (FLAS)</v>
+        <v>A. M. Brenes s. n. (NY)</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>432</v>
+      <c r="B42" s="16" t="s">
+        <v>245</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D42" s="6" t="s">
-        <v>213</v>
+      <c r="D42" s="10" t="s">
+        <v>444</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>410</v>
+        <v>330</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
-        <v>A. M. Brenes s. n. (NY)</v>
+        <v>A. Charpin et al. s. n. (NY)</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>248</v>
+      <c r="B43" s="16" t="s">
+        <v>246</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="10"/>
+      <c r="D43" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E43" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>335</v>
+        <v>406</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
-        <v>A. Charpin et al. s. n. (NY)</v>
+        <v>S. K. Lau 1915 (NY)</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
-      <c r="B44" s="11" t="s">
-        <v>249</v>
+      <c r="B44" s="15" t="s">
+        <v>247</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D44" s="6"/>
+      <c r="D44" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E44" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v>S. K. Lau 1915 (NY)</v>
+        <v>G. F. Buddell II 2352 (NY)</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>250</v>
+      <c r="B45" s="18" t="s">
+        <v>248</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>4</v>
+      <c r="D45" s="10" t="s">
+        <v>444</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>412</v>
+        <v>334</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
-        <v>G. F. Buddell II 2352 (NY)</v>
+        <v>J. C. Arthwz s. n. (NY)</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
-      <c r="B46" s="19"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E46" s="12" t="s">
-        <v>424</v>
+      <c r="E46" s="11" t="s">
+        <v>419</v>
       </c>
       <c r="G46" s="5"/>
       <c r="H46" t="str">
@@ -5104,304 +5189,330 @@
       <c r="A47" s="5">
         <v>46</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>251</v>
+      <c r="B47" s="16" t="s">
+        <v>249</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D47" s="10"/>
+      <c r="D47" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="E47" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>J. C. Arthwz s. n. (NY)</v>
+        <v>L. Maplcoba s. n. (NY)</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="19"/>
+      <c r="B48" s="16" t="s">
+        <v>250</v>
+      </c>
       <c r="C48" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="G48" s="5"/>
+        <v>213</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>338</v>
+      </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>Herbarium name not recognized</v>
+        <v>J. J. Castillo &amp; J. M. Vargas 2722 (NY)</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
-      <c r="B49" s="11" t="s">
-        <v>252</v>
+      <c r="B49" s="16" t="s">
+        <v>251</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D49" s="10"/>
+      <c r="D49" s="6" t="s">
+        <v>444</v>
+      </c>
       <c r="E49" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F49" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="G49" s="5" t="s">
-        <v>341</v>
-      </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>L. Maplcoba s. n. (NY)</v>
+        <v>Jorge A. Molina 30005 (NY)</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>
-      <c r="B50" s="11" t="s">
-        <v>253</v>
+      <c r="B50" s="16" t="s">
+        <v>252</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D50" s="10" t="s">
         <v>213</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F50" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="G50" s="5" t="s">
-        <v>343</v>
-      </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>J. J. Castillo &amp; J. M. Vargas 2722 (NY)</v>
+        <v>Hinton et al. 21760 (NY)</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>50</v>
       </c>
-      <c r="B51" s="11" t="s">
-        <v>254</v>
+      <c r="B51" s="16" t="s">
+        <v>253</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D51" s="6"/>
+      <c r="D51" s="10" t="s">
+        <v>212</v>
+      </c>
       <c r="E51" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F51" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="G51" s="5" t="s">
-        <v>345</v>
-      </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>Jorge A. Molina 30005 (NY)</v>
+        <v>H. D. Ripley 14966 (NY)</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>51</v>
       </c>
-      <c r="B52" s="11" t="s">
-        <v>255</v>
+      <c r="B52" s="16" t="s">
+        <v>254</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D52" s="10" t="s">
-        <v>213</v>
+      <c r="D52" s="6" t="s">
+        <v>444</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F52" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="G52" s="5" t="s">
-        <v>347</v>
-      </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>Hinton et al. 21760 (NY)</v>
+        <v>Assadi, Edmondson &amp; Miller 2135 (NY)</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>52</v>
       </c>
-      <c r="B53" s="11" t="s">
-        <v>256</v>
+      <c r="B53" s="18" t="s">
+        <v>255</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D53" s="10" t="s">
-        <v>212</v>
+      <c r="D53" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>349</v>
+        <v>408</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
-        <v>H. D. Ripley 14966 (NY)</v>
+        <v>D. S. Correll &amp; H. B. Correll 51703 (NY)</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>53</v>
       </c>
-      <c r="B54" s="11" t="s">
-        <v>257</v>
-      </c>
+      <c r="B54" s="18"/>
       <c r="C54" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D54" s="6"/>
+      <c r="D54" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E54" s="6" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>351</v>
+        <v>452</v>
+      </c>
+      <c r="G54" s="19" t="s">
+        <v>453</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
-        <v>Assadi, Edmondson &amp; Miller 2135 (NY)</v>
+        <v>Hillary M. Cherry 270 (FLAS)</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>54</v>
       </c>
-      <c r="B55" s="11" t="s">
-        <v>258</v>
+      <c r="B55" s="16" t="s">
+        <v>256</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D55" s="6"/>
+      <c r="D55" s="6" t="s">
+        <v>444</v>
+      </c>
       <c r="E55" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>413</v>
+        <v>349</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>D. S. Correll &amp; H. B. Correll 51703 (NY)</v>
+        <v>C. L. Lundell 14978 (NY)</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>55</v>
       </c>
-      <c r="B56" s="11" t="s">
-        <v>258</v>
+      <c r="B56" s="16" t="s">
+        <v>257</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D56" s="6"/>
+      <c r="D56" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E56" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="G56" s="13"/>
+        <v>390</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>351</v>
+      </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> (FLAS)</v>
+        <v>L. H. Cramer 4871 (NY)</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>56</v>
       </c>
-      <c r="B57" s="11" t="s">
-        <v>259</v>
+      <c r="B57" s="16" t="s">
+        <v>258</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D57" s="6"/>
+      <c r="D57" s="10" t="s">
+        <v>213</v>
+      </c>
       <c r="E57" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F57" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="G57" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="G57" s="5" t="s">
-        <v>354</v>
-      </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
-        <v>C. L. Lundell 14978 (NY)</v>
+        <v>E. Serowa &amp; E. Ryschowa s. n. (NY)</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>57</v>
       </c>
-      <c r="B58" s="11" t="s">
-        <v>260</v>
+      <c r="B58" s="16" t="s">
+        <v>259</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D58" s="6"/>
+      <c r="D58" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="E58" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>356</v>
+        <v>409</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
-        <v>L. H. Cramer 4871 (NY)</v>
+        <v>R. D. Thomas et al. 170488 (NY)</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>58</v>
       </c>
-      <c r="B59" s="11" t="s">
-        <v>261</v>
+      <c r="B59" s="16" t="s">
+        <v>260</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>207</v>
@@ -5410,501 +5521,528 @@
         <v>213</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>358</v>
+        <v>410</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
-        <v>E. Serowa &amp; E. Ryschowa s. n. (NY)</v>
+        <v>R. D. Thomas &amp; C. Slaughter 103883 (NY)</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>59</v>
       </c>
-      <c r="B60" s="11" t="s">
-        <v>262</v>
+      <c r="B60" s="16" t="s">
+        <v>261</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D60" s="10" t="s">
-        <v>4</v>
+      <c r="D60" s="6" t="s">
+        <v>444</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
-        <v>R. D. Thomas et al. 170488 (NY)</v>
+        <v>P. Jaeger 8796 (NY)</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>60</v>
       </c>
-      <c r="B61" s="11" t="s">
-        <v>263</v>
+      <c r="B61" s="16" t="s">
+        <v>424</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>360</v>
+        <v>393</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>415</v>
+        <v>423</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
-        <v>R. D. Thomas &amp; C. Slaughter 103883 (NY)</v>
+        <v>S. Kim 2015-0268 (SWU)</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>61</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>264</v>
+      <c r="B62" s="16" t="s">
+        <v>262</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D62" s="6"/>
+      <c r="D62" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E62" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
-        <v>P. Jaeger 8796 (NY)</v>
+        <v>H. Field &amp; Y. Lazar s. n. (NY)</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>62</v>
       </c>
-      <c r="B63" s="11" t="s">
-        <v>429</v>
+      <c r="B63" s="16" t="s">
+        <v>263</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>212</v>
+        <v>207</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>444</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>398</v>
+        <v>390</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>358</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>428</v>
+        <v>359</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
-        <v>S. Kim 2015-0268 (SWU)</v>
+        <v>K. H. Rechinger 686 (NY)</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>63</v>
       </c>
-      <c r="B64" s="11" t="s">
-        <v>265</v>
+      <c r="B64" s="16" t="s">
+        <v>264</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D64" s="6"/>
+      <c r="D64" s="10" t="s">
+        <v>213</v>
+      </c>
       <c r="E64" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v>H. Field &amp; Y. Lazar s. n. (NY)</v>
+        <v>D. S. Correll &amp; H. B. Correll 30562 (NY)</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>64</v>
       </c>
-      <c r="B65" s="11" t="s">
-        <v>266</v>
+      <c r="B65" s="16" t="s">
+        <v>265</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D65" s="6"/>
+      <c r="D65" s="6" t="s">
+        <v>444</v>
+      </c>
       <c r="E65" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>364</v>
+        <v>413</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" si="0"/>
-        <v>K. H. Rechinger 686 (NY)</v>
+        <f t="shared" ref="H65:H83" si="2">IF(E65="Steere Herbarium, NY, USA", CONCATENATE(G65, " (NY)"), IF(E65="University of Florida Herbarium, FL, USA", CONCATENATE(G65, " (FLAS)"), IF(E65="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G65, " (SWU)"), "Herbarium name not recognized")))</f>
+        <v>W. Koelz 21180 (NY)</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>65</v>
       </c>
-      <c r="B66" s="11" t="s">
-        <v>267</v>
+      <c r="B66" s="16" t="s">
+        <v>266</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D66" s="10" t="s">
-        <v>213</v>
+      <c r="D66" s="6" t="s">
+        <v>444</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>417</v>
+        <v>363</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" si="0"/>
-        <v>D. S. Correll &amp; H. B. Correll 30562 (NY)</v>
+        <f t="shared" si="2"/>
+        <v>L. Janczenko s. n. (NY)</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>66</v>
       </c>
-      <c r="B67" s="11" t="s">
-        <v>268</v>
+      <c r="B67" s="16" t="s">
+        <v>267</v>
       </c>
       <c r="C67" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D67" s="6"/>
+      <c r="D67" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E67" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>418</v>
+        <v>317</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" ref="H67:H85" si="1">IF(E67="Steere Herbarium, NY, USA", CONCATENATE(G67, " (NY)"), IF(E67="University of Florida Herbarium, FL, USA", CONCATENATE(G67, " (FLAS)"), IF(E67="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G67, " (SWU)"), "Herbarium name not recognized")))</f>
-        <v>W. Koelz 21180 (NY)</v>
+        <f t="shared" si="2"/>
+        <v>R. Kral s. n. (NY)</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>67</v>
       </c>
-      <c r="B68" s="11" t="s">
-        <v>269</v>
+      <c r="B68" s="16" t="s">
+        <v>268</v>
       </c>
       <c r="C68" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D68" s="6"/>
+      <c r="D68" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="E68" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H68" t="str">
-        <f t="shared" si="1"/>
-        <v>L. Janczenko s. n. (NY)</v>
+        <f t="shared" si="2"/>
+        <v>R. Schischkin et al. s. n. (NY)</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>68</v>
       </c>
-      <c r="B69" s="11" t="s">
-        <v>270</v>
+      <c r="B69" s="16" t="s">
+        <v>269</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D69" s="6"/>
+      <c r="D69" s="6" t="s">
+        <v>444</v>
+      </c>
       <c r="E69" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>320</v>
+        <v>405</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" si="1"/>
-        <v>R. Kral s. n. (NY)</v>
+        <f t="shared" si="2"/>
+        <v>A. M. Brenes s. n. (NY)</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>69</v>
       </c>
-      <c r="B70" s="11" t="s">
-        <v>271</v>
+      <c r="B70" s="18" t="s">
+        <v>270</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D70" s="10" t="s">
-        <v>2</v>
+      <c r="D70" s="6" t="s">
+        <v>444</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>371</v>
+        <v>454</v>
+      </c>
+      <c r="G70" s="19" t="s">
+        <v>455</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="1"/>
-        <v>R. Schischkin et al. s. n. (NY)</v>
+        <f t="shared" si="2"/>
+        <v>s. n. (FLAS)</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>70</v>
       </c>
-      <c r="B71" s="11" t="s">
-        <v>272</v>
-      </c>
+      <c r="B71" s="18"/>
       <c r="C71" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>410</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="G71" s="5"/>
       <c r="H71" t="str">
-        <f t="shared" si="1"/>
-        <v>A. M. Brenes s. n. (NY)</v>
+        <f t="shared" si="2"/>
+        <v>Herbarium name not recognized</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>71</v>
       </c>
-      <c r="B72" s="19" t="s">
-        <v>273</v>
+      <c r="B72" s="16" t="s">
+        <v>271</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D72" s="6"/>
+      <c r="D72" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="E72" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="G72" s="13"/>
+        <v>390</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>369</v>
+      </c>
       <c r="H72" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> (FLAS)</v>
+        <f t="shared" si="2"/>
+        <v>A. Donmez 3627 (NY)</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>72</v>
       </c>
-      <c r="B73" s="19"/>
+      <c r="B73" s="16" t="s">
+        <v>272</v>
+      </c>
       <c r="C73" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="E73" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="G73" s="5"/>
+        <v>213</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>414</v>
+      </c>
       <c r="H73" t="str">
-        <f t="shared" si="1"/>
-        <v>Herbarium name not recognized</v>
+        <f t="shared" si="2"/>
+        <v>G. C. Freeman &amp; R. E. Brooks 3682 (NY)</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>73</v>
       </c>
-      <c r="B74" s="11" t="s">
-        <v>274</v>
+      <c r="B74" s="16" t="s">
+        <v>273</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D74" s="6"/>
+      <c r="D74" s="10" t="s">
+        <v>213</v>
+      </c>
       <c r="E74" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H74" t="str">
-        <f t="shared" si="1"/>
-        <v>A. Donmez 3627 (NY)</v>
+        <f t="shared" si="2"/>
+        <v>S. L. Welsh 20585 (NY)</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>74</v>
       </c>
-      <c r="B75" s="11" t="s">
-        <v>275</v>
+      <c r="B75" s="16" t="s">
+        <v>274</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D75" s="10" t="s">
-        <v>213</v>
+      <c r="D75" s="6" t="s">
+        <v>444</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>419</v>
+        <v>374</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="1"/>
-        <v>G. C. Freeman &amp; R. E. Brooks 3682 (NY)</v>
+        <f t="shared" si="2"/>
+        <v>H. H. Iltis et al. 307 (NY)</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>75</v>
       </c>
-      <c r="B76" s="11" t="s">
-        <v>276</v>
+      <c r="B76" s="16" t="s">
+        <v>275</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D76" s="10" t="s">
-        <v>213</v>
+      <c r="D76" s="6" t="s">
+        <v>444</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F76" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="G76" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="G76" s="5" t="s">
-        <v>377</v>
-      </c>
       <c r="H76" t="str">
-        <f t="shared" si="1"/>
-        <v>S. L. Welsh 20585 (NY)</v>
+        <f t="shared" si="2"/>
+        <v>C. G. Pringle s. n. (NY)</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>76</v>
       </c>
-      <c r="B77" s="11" t="s">
-        <v>277</v>
+      <c r="B77" s="16" t="s">
+        <v>276</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D77" s="6"/>
+      <c r="D77" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="E77" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F77" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="G77" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="G77" s="5" t="s">
-        <v>379</v>
-      </c>
       <c r="H77" t="str">
-        <f t="shared" si="1"/>
-        <v>H. H. Iltis et al. 307 (NY)</v>
+        <f t="shared" si="2"/>
+        <v>J. J. Carter s. n. (NY)</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>77</v>
       </c>
-      <c r="B78" s="11" t="s">
-        <v>278</v>
+      <c r="B78" s="16" t="s">
+        <v>277</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D78" s="6"/>
+      <c r="D78" s="10" t="s">
+        <v>213</v>
+      </c>
       <c r="E78" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>381</v>
+        <v>415</v>
       </c>
       <c r="H78" t="str">
-        <f t="shared" si="1"/>
-        <v>C. G. Pringle s. n. (NY)</v>
+        <f t="shared" si="2"/>
+        <v>S. D. White 4380 (NY)</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>78</v>
       </c>
-      <c r="B79" s="11" t="s">
-        <v>279</v>
+      <c r="B79" s="16" t="s">
+        <v>278</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>207</v>
@@ -5913,248 +6051,192 @@
         <v>4</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H79" t="str">
-        <f t="shared" si="1"/>
-        <v>J. J. Carter s. n. (NY)</v>
+        <f t="shared" si="2"/>
+        <v>A. Villegas H. 00063 (NY)</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>79</v>
       </c>
-      <c r="B80" s="11" t="s">
-        <v>280</v>
+      <c r="B80" s="16" t="s">
+        <v>279</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="H80" t="str">
-        <f t="shared" si="1"/>
-        <v>S. D. White 4380 (NY)</v>
+        <f t="shared" si="2"/>
+        <v>S. Kim 20140705 (SWU)</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>80</v>
       </c>
-      <c r="B81" s="11" t="s">
-        <v>281</v>
+      <c r="B81" s="16" t="s">
+        <v>280</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D81" s="10" t="s">
-        <v>4</v>
+      <c r="D81" s="6" t="s">
+        <v>444</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>386</v>
+        <v>416</v>
       </c>
       <c r="H81" t="str">
-        <f t="shared" si="1"/>
-        <v>A. Villegas H. 00063 (NY)</v>
+        <f t="shared" si="2"/>
+        <v>J. L. Reveal 3390 (NY)</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>81</v>
       </c>
-      <c r="B82" s="11" t="s">
-        <v>282</v>
+      <c r="B82" s="16" t="s">
+        <v>281</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D82" s="10" t="s">
-        <v>212</v>
+        <v>207</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>398</v>
+        <v>390</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>383</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="H82" t="str">
-        <f t="shared" si="1"/>
-        <v>S. Kim 20140705 (SWU)</v>
+        <f t="shared" si="2"/>
+        <v>C. Hamel &amp; R. S. Toroes 767 (NY)</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>82</v>
       </c>
-      <c r="B83" s="11" t="s">
-        <v>283</v>
+      <c r="B83" s="16" t="s">
+        <v>282</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D83" s="6"/>
+      <c r="D83" s="10" t="s">
+        <v>213</v>
+      </c>
       <c r="E83" s="6" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>421</v>
+        <v>385</v>
       </c>
       <c r="H83" t="str">
-        <f t="shared" si="1"/>
-        <v>J. L. Reveal 3390 (NY)</v>
+        <f t="shared" si="2"/>
+        <v>R. D. Worthington 13323 (NY)</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>83</v>
       </c>
-      <c r="B84" s="11" t="s">
-        <v>284</v>
+      <c r="B84" s="16" t="s">
+        <v>283</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D84" s="6"/>
-      <c r="E84" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>422</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E84" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="G84" s="5"/>
       <c r="H84" t="str">
-        <f t="shared" si="1"/>
-        <v>C. Hamel &amp; R. S. Toroes 767 (NY)</v>
+        <f>IF(E84="Steere Herbarium, NY, USA", CONCATENATE(G84, " (NY)"), IF(E84="University of Florida Herbarium, FL, USA", CONCATENATE(G84, " (FLAS)"), IF(E84="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G84, " (SWU)"), "Herbarium name not recognized")))</f>
+        <v>Herbarium name not recognized</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>84</v>
       </c>
-      <c r="B85" s="11" t="s">
-        <v>285</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D85" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="G85" s="5" t="s">
-        <v>390</v>
-      </c>
+      <c r="B85" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="F85"/>
       <c r="H85" t="str">
-        <f t="shared" si="1"/>
-        <v>R. D. Worthington 13323 (NY)</v>
+        <f>IF(E85="Steere Herbarium, NY, USA", CONCATENATE(G85, " (NY)"), IF(E85="University of Florida Herbarium, FL, USA", CONCATENATE(G85, " (FLAS)"), IF(E85="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G85, " (SWU)"), "Herbarium name not recognized")))</f>
+        <v>Herbarium name not recognized</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="5">
-        <v>85</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D86" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="E86" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="G86" s="5"/>
-      <c r="H86" t="str">
-        <f>IF(E86="Steere Herbarium, NY, USA", CONCATENATE(G86, " (NY)"), IF(E86="University of Florida Herbarium, FL, USA", CONCATENATE(G86, " (FLAS)"), IF(E86="Sungshin Herbarium, Seoul, Republic of Korea", CONCATENATE(G86, " (SWU)"), "Herbarium name not recognized")))</f>
-        <v>Herbarium name not recognized</v>
-      </c>
+      <c r="F86"/>
     </row>
     <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F87"/>
+      <c r="B87" s="13"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="11"/>
     </row>
     <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="15" t="s">
-        <v>433</v>
-      </c>
-      <c r="C88" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="D88" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="E88" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="F88"/>
-    </row>
-    <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="15" t="s">
-        <v>434</v>
-      </c>
-      <c r="C89" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="D89" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="E89" s="12" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="C90" s="16" t="s">
-        <v>207</v>
-      </c>
+      <c r="B88" s="13"/>
+      <c r="C88" s="14"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E87">
-    <sortCondition ref="B2:B87"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E85">
+    <sortCondition ref="B2:B85"/>
   </sortState>
-  <mergeCells count="7">
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B9:B10"/>
+  <mergeCells count="6">
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B70:B71"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B53:B54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="25" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -6191,20 +6273,20 @@
         <v>211</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>215</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -6214,14 +6296,14 @@
         <v>212</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>220</v>
+      <c r="A3" s="15" t="s">
+        <v>219</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>206</v>
@@ -6230,14 +6312,14 @@
         <v>212</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>222</v>
+      <c r="A4" s="12" t="s">
+        <v>221</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>206</v>
@@ -6246,13 +6328,13 @@
         <v>212</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="6"/>
@@ -6260,8 +6342,8 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>239</v>
+      <c r="A6" s="15" t="s">
+        <v>238</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>206</v>
@@ -6270,13 +6352,13 @@
         <v>212</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="6"/>
@@ -6284,8 +6366,8 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>251</v>
+      <c r="A8" s="15" t="s">
+        <v>248</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>206</v>
@@ -6294,14 +6376,14 @@
         <v>212</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>273</v>
+      <c r="A9" s="15" t="s">
+        <v>270</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>206</v>
@@ -6310,14 +6392,14 @@
         <v>212</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>286</v>
+      <c r="A10" s="12" t="s">
+        <v>283</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>206</v>
@@ -6326,23 +6408,23 @@
         <v>212</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>433</v>
-      </c>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="14" t="s">
         <v>212</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>